<commit_message>
Sirenum ep 4 prep
</commit_message>
<xml_diff>
--- a/mars_habs.xlsx
+++ b/mars_habs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
   <si>
     <t>Location</t>
   </si>
@@ -389,6 +389,105 @@
   </si>
   <si>
     <t>ORB 2</t>
+  </si>
+  <si>
+    <t>Tharsis TH</t>
+  </si>
+  <si>
+    <t>Valles Map</t>
+  </si>
+  <si>
+    <t>Terraforming hub</t>
+  </si>
+  <si>
+    <t>Eos TH</t>
+  </si>
+  <si>
+    <t>Eos Chasma</t>
+  </si>
+  <si>
+    <t>Mellas TH</t>
+  </si>
+  <si>
+    <t>Calaiâ</t>
+  </si>
+  <si>
+    <t>Melas Chasma</t>
+  </si>
+  <si>
+    <t>Aquatic uplifts</t>
+  </si>
+  <si>
+    <t>Fields of Steel</t>
+  </si>
+  <si>
+    <t>Solis Planum</t>
+  </si>
+  <si>
+    <t>Industrial town</t>
+  </si>
+  <si>
+    <t>Portmanteau</t>
+  </si>
+  <si>
+    <t>Hyblaeus</t>
+  </si>
+  <si>
+    <t>Rangers</t>
+  </si>
+  <si>
+    <t>SW121</t>
+  </si>
+  <si>
+    <t>Base of Portmanteau Rangers</t>
+  </si>
+  <si>
+    <t>Langlac</t>
+  </si>
+  <si>
+    <t>Orcus Patera</t>
+  </si>
+  <si>
+    <t>Elysium Map</t>
+  </si>
+  <si>
+    <t>Former tourist destination</t>
+  </si>
+  <si>
+    <t>Cerberus Fossae</t>
+  </si>
+  <si>
+    <t>Economic outpost</t>
+  </si>
+  <si>
+    <t>Argoed</t>
+  </si>
+  <si>
+    <t>Utopia Plaintia</t>
+  </si>
+  <si>
+    <t>Former quarry, now growing hub</t>
+  </si>
+  <si>
+    <t>LL 1-2</t>
+  </si>
+  <si>
+    <t>Eddie</t>
+  </si>
+  <si>
+    <t>UTO</t>
+  </si>
+  <si>
+    <t>Todor</t>
+  </si>
+  <si>
+    <t>Louros Valles</t>
+  </si>
+  <si>
+    <t>Railway Infra Town</t>
+  </si>
+  <si>
+    <t>Eos Rail, IWA</t>
   </si>
 </sst>
 </file>
@@ -772,7 +871,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -780,11 +879,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,7 +959,7 @@
         <v>0.4</v>
       </c>
       <c r="I2" s="10">
-        <f t="shared" ref="I2:I30" si="0">G2*H2</f>
+        <f t="shared" ref="I2:I40" si="0">G2*H2</f>
         <v>14800000</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -946,7 +1045,7 @@
       </c>
       <c r="L5" s="3">
         <f>SUM(G1:G124)</f>
-        <v>72638300</v>
+        <v>74403300</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -1011,260 +1110,269 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3">
+        <v>600000</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="J8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>91</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="3">
         <v>350000</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="7">
         <v>0.25</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I9" s="10">
         <f t="shared" si="0"/>
         <v>87500</v>
       </c>
-      <c r="L8" s="3">
-        <f>SUM(I2:I124)</f>
-        <v>27969370</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="3">
-        <v>300000</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.45</v>
-      </c>
-      <c r="I9" s="10">
-        <f t="shared" si="0"/>
-        <v>135000</v>
+      <c r="L9" s="3">
+        <f>SUM(I3:I125)</f>
+        <v>14054870</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="G10" s="3">
-        <v>120000</v>
+        <v>300000</v>
       </c>
       <c r="H10" s="7">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="0"/>
-        <v>84000</v>
-      </c>
-      <c r="J10" t="s">
-        <v>78</v>
+        <v>135000</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1">
       <c r="A11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
+        <v>124</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="E11"/>
       <c r="F11" s="4" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="G11" s="3">
+        <v>300000</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-      <c r="H11" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="I11" s="10">
-        <f t="shared" si="0"/>
-        <v>54000</v>
-      </c>
-      <c r="J11"/>
-      <c r="L11" t="s">
-        <v>76</v>
-      </c>
+      <c r="J11" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>101</v>
+        <v>145</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3">
-        <v>30000</v>
+        <v>160000</v>
       </c>
       <c r="H12" s="7">
         <v>0.6</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="0"/>
-        <v>18000</v>
+        <v>96000</v>
+      </c>
+      <c r="J12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="4" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>131</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="G13" s="3">
-        <v>30000</v>
+        <v>140000</v>
       </c>
       <c r="H13" s="7">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
-        <v>15000</v>
+        <v>84000</v>
       </c>
       <c r="J13" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="4" t="s">
-        <v>93</v>
+        <v>121</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>114</v>
+        <v>68</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="3">
-        <v>25000</v>
+        <v>130000</v>
       </c>
       <c r="H14" s="7">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="I14" s="10">
         <f t="shared" si="0"/>
-        <v>13750.000000000002</v>
+        <v>78000</v>
+      </c>
+      <c r="J14" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
+        <v>92</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="G15" s="3">
-        <v>25000</v>
+        <v>120000</v>
       </c>
       <c r="H15" s="7">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="I15" s="10">
         <f t="shared" si="0"/>
-        <v>16250</v>
+        <v>84000</v>
       </c>
       <c r="J15" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="4" customFormat="1">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
+      <c r="A16" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="G16" s="3">
-        <v>10000</v>
+        <v>120000</v>
       </c>
       <c r="H16" s="7">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="I16" s="10">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>72000</v>
       </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>149</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>
@@ -1272,407 +1380,701 @@
       <c r="N16"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="A17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>95000</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="0"/>
+        <v>47500</v>
+      </c>
+      <c r="J17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="3">
+        <v>90000</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="0"/>
+        <v>54000</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="L18" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="3">
+        <v>80000</v>
+      </c>
+      <c r="H19" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="0"/>
+        <v>32000</v>
+      </c>
+      <c r="J19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="3">
-        <v>8000</v>
-      </c>
-      <c r="H17" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I17" s="10">
-        <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="3">
-        <v>7500</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I18" s="10">
-        <f t="shared" si="0"/>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="3">
-        <v>6000</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="I19" s="10">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="M19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" t="s">
-        <v>32</v>
-      </c>
       <c r="G20" s="3">
-        <v>6000</v>
+        <v>80000</v>
       </c>
       <c r="H20" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="I20" s="10">
         <f t="shared" si="0"/>
-        <v>4800</v>
-      </c>
-      <c r="M20" t="s">
-        <v>12</v>
-      </c>
-      <c r="N20">
-        <f>COUNTIF(D3:D1002,"*D*")+COUNTIF(D3:D1002,"DD*")+COUNTIF(D3:D1002,"DDD")</f>
-        <v>0</v>
+        <v>56000</v>
+      </c>
+      <c r="J20" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
+        <v>127</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" t="s">
-        <v>117</v>
+      <c r="D21" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="G21" s="3">
-        <v>5500</v>
+        <v>60000</v>
       </c>
       <c r="H21" s="7">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I21" s="10">
         <f t="shared" si="0"/>
-        <v>4950</v>
-      </c>
-      <c r="M21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21">
-        <f>COUNTIF(D3:D102,"*X*")+COUNTIF(D3:D102,"XX*")+COUNTIF(D3:D1002,"XXX")</f>
-        <v>0</v>
+        <v>30000</v>
+      </c>
+      <c r="J21" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" t="s">
-        <v>25</v>
+      <c r="A22" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H23" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="J23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="3">
+        <v>25000</v>
+      </c>
+      <c r="H24" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="0"/>
+        <v>13750.000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H22" s="7">
+      <c r="G25" s="3">
+        <v>25000</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="0"/>
+        <v>16250</v>
+      </c>
+      <c r="J25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H26" s="7">
         <v>0.3</v>
       </c>
-      <c r="I22" s="10">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="I26" s="10">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="J26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H23" s="7">
+      <c r="G27" s="3">
+        <v>8000</v>
+      </c>
+      <c r="H27" s="7">
         <v>0.3</v>
       </c>
-      <c r="I23" s="10">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="J23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" t="s">
-        <v>14</v>
-      </c>
-      <c r="N23">
-        <f>COUNTIF(D3:D102,"*F*")+COUNTIF(D3:D102,"FF*")+COUNTIF(D3:D1002,"FFF")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="I27" s="10">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H24" s="7">
+      <c r="G28" s="3">
+        <v>7500</v>
+      </c>
+      <c r="H28" s="7">
         <v>0.3</v>
       </c>
-      <c r="I24" s="10">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="J24" t="s">
-        <v>36</v>
-      </c>
-      <c r="M24" t="s">
-        <v>15</v>
-      </c>
-      <c r="N24">
-        <f>COUNTIF(D3:D102,"*R*")+COUNTIF(D3:D102,"RR*")+COUNTIF(D3:D1002,"RRR")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="I25" s="10">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1700</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="I26" s="10">
-        <f t="shared" si="0"/>
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="3">
-        <v>1000</v>
-      </c>
-      <c r="H27" s="7">
-        <v>0.8</v>
-      </c>
-      <c r="I27" s="10">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="J27" t="s">
-        <v>44</v>
-      </c>
-      <c r="M27" t="s">
-        <v>10</v>
-      </c>
-      <c r="N27">
-        <f>SUM(N20:N26)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1000</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0.9</v>
-      </c>
       <c r="I28" s="10">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="4" t="s">
-        <v>74</v>
+      <c r="A29" t="s">
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>5</v>
+        <v>84</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
       </c>
       <c r="G29" s="3">
-        <v>900</v>
+        <v>6000</v>
       </c>
       <c r="H29" s="7">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="I29" s="10">
         <f t="shared" si="0"/>
-        <v>810</v>
+        <v>1800</v>
+      </c>
+      <c r="M29" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
         <v>34</v>
       </c>
       <c r="E30" t="s">
         <v>101</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="3">
+        <v>6000</v>
+      </c>
+      <c r="H30" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="I30" s="10">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+      <c r="M30" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30">
+        <f>COUNTIF(D13:D1012,"*D*")+COUNTIF(D13:D1012,"DD*")+COUNTIF(D13:D1012,"DDD")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="3">
+        <v>5500</v>
+      </c>
+      <c r="H31" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="I31" s="10">
+        <f t="shared" si="0"/>
+        <v>4950</v>
+      </c>
+      <c r="M31" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31">
+        <f>COUNTIF(D13:D112,"*X*")+COUNTIF(D13:D112,"XX*")+COUNTIF(D13:D1012,"XXX")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I32" s="10">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="J33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M33" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33">
+        <f>COUNTIF(D13:D112,"*F*")+COUNTIF(D13:D112,"FF*")+COUNTIF(D13:D1012,"FFF")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="I34" s="10">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="J34" t="s">
+        <v>36</v>
+      </c>
+      <c r="M34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34">
+        <f>COUNTIF(D13:D112,"*R*")+COUNTIF(D13:D112,"RR*")+COUNTIF(D13:D1012,"RRR")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="I35" s="10">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G36" s="3">
+        <v>1700</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="10">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H37" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="I37" s="10">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="J37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37">
+        <f>SUM(N30:N36)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" t="s">
+        <v>117</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H38" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="I38" s="10">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="3">
+        <v>900</v>
+      </c>
+      <c r="H39" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="I39" s="10">
+        <f t="shared" si="0"/>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="5">
         <v>700</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H40" s="8">
         <v>0.7</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I40" s="10">
         <f t="shared" si="0"/>
         <v>489.99999999999994</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J40" s="4" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:N30">
-    <sortCondition descending="1" ref="G1:G30"/>
+  <sortState ref="A1:N40">
+    <sortCondition descending="1" ref="G1:G40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updates after Sirenum 004
</commit_message>
<xml_diff>
--- a/mars_habs.xlsx
+++ b/mars_habs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="152">
   <si>
     <t>Location</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>Eos Rail, IWA</t>
+  </si>
+  <si>
+    <t>Triolet Community</t>
   </si>
 </sst>
 </file>
@@ -871,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -879,11 +882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -959,7 +962,7 @@
         <v>0.4</v>
       </c>
       <c r="I2" s="10">
-        <f t="shared" ref="I2:I40" si="0">G2*H2</f>
+        <f>G2*H2</f>
         <v>14800000</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -986,7 +989,7 @@
         <v>0.45</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I3:I41" si="0">G3*H3</f>
         <v>5850000</v>
       </c>
     </row>
@@ -1045,7 +1048,7 @@
       </c>
       <c r="L5" s="3">
         <f>SUM(G1:G124)</f>
-        <v>74403300</v>
+        <v>74403450</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -1167,7 +1170,7 @@
       </c>
       <c r="L9" s="3">
         <f>SUM(I3:I125)</f>
-        <v>14054870</v>
+        <v>14054907.5</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1897,7 +1900,7 @@
       </c>
       <c r="N34">
         <f>COUNTIF(D13:D112,"*R*")+COUNTIF(D13:D112,"RR*")+COUNTIF(D13:D1012,"RRR")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1979,7 +1982,7 @@
       </c>
       <c r="N37">
         <f>SUM(N30:N36)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2069,6 +2072,39 @@
         <v>489.99999999999994</v>
       </c>
       <c r="J40" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="3">
+        <v>150</v>
+      </c>
+      <c r="H41" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="I41" s="10">
+        <f t="shared" si="0"/>
+        <v>37.5</v>
+      </c>
+      <c r="J41" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update out there 008
</commit_message>
<xml_diff>
--- a/mars_habs.xlsx
+++ b/mars_habs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="3460" windowWidth="28800" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hab populations" sheetId="2" r:id="rId1"/>
@@ -886,7 +886,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="L5" s="3">
         <f>SUM(G1:G124)</f>
-        <v>74403450</v>
+        <v>74423450</v>
       </c>
       <c r="N5" s="3"/>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="L9" s="3">
         <f>SUM(I3:I125)</f>
-        <v>14054907.5</v>
+        <v>14056907.5</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1555,14 +1555,14 @@
         <v>81</v>
       </c>
       <c r="G22" s="3">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="H22" s="7">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="I22" s="10">
         <f t="shared" si="0"/>
-        <v>18000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="23" spans="1:14">

</xml_diff>